<commit_message>
Made changes to reports generation and removed prj packages.
</commit_message>
<xml_diff>
--- a/src/test/resources/com/Demo/mobile/login/testdata/Login.xlsx
+++ b/src/test/resources/com/Demo/mobile/login/testdata/Login.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10210"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20228"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B403260D-5689-49B3-B21C-74BC20A08681}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="462" windowWidth="25602" windowHeight="14640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="11" r:id="rId1"/>
@@ -487,20 +488,20 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="10.1640625" customWidth="1"/>
-    <col min="2" max="2" width="15.1640625" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" customWidth="1"/>
-    <col min="4" max="4" width="15.5" customWidth="1"/>
-    <col min="5" max="5" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.5" customWidth="1"/>
+    <col min="1" max="1" width="10.15625" customWidth="1"/>
+    <col min="2" max="2" width="15.15625" customWidth="1"/>
+    <col min="3" max="3" width="14.3125" customWidth="1"/>
+    <col min="4" max="4" width="15.47265625" customWidth="1"/>
+    <col min="5" max="5" width="25.3125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.47265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
@@ -517,7 +518,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -534,7 +535,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -551,35 +552,35 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" s="1"/>
     </row>
   </sheetData>
@@ -600,13 +601,13 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.9453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="4" max="4" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.47265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.47265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
@@ -629,7 +630,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -652,7 +653,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -675,7 +676,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -698,7 +699,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -721,7 +722,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -742,7 +743,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>8</v>
       </c>

</xml_diff>